<commit_message>
just before adding changes
</commit_message>
<xml_diff>
--- a/data/CEA_Estimates.xlsx
+++ b/data/CEA_Estimates.xlsx
@@ -7,14 +7,15 @@
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Display" sheetId="1" r:id="rId1"/>
+    <sheet name="Work" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="17">
   <si>
     <t>Mortality</t>
   </si>
@@ -43,22 +44,34 @@
     <t>Estimate for 2015 (CEA)</t>
   </si>
   <si>
-    <t>$431.7 billion</t>
-  </si>
-  <si>
-    <t>$36.6 billion</t>
-  </si>
-  <si>
-    <t>$25.9 billion</t>
-  </si>
-  <si>
-    <t>$9.7 billion</t>
+    <t>Updated Estimates (2017 dollars)</t>
+  </si>
+  <si>
+    <t>Weights</t>
+  </si>
+  <si>
+    <t>Non-productivity pp (2015 dollars)</t>
+  </si>
+  <si>
+    <t>Non-productivity pp (2017 dollars)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Updated Updated 2017 Estimates </t>
+  </si>
+  <si>
+    <t>Percent Cost Change</t>
+  </si>
+  <si>
+    <t>Total non-productivity (2017 Millions)</t>
+  </si>
+  <si>
+    <t>2015 CEA Estimate (2017 Dollars)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -394,15 +407,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -410,51 +423,226 @@
         <v>3</v>
       </c>
       <c r="C1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+      <c r="D1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C2">
+        <f>431.7*1.04</f>
+        <v>448.96800000000002</v>
+      </c>
+      <c r="D2">
+        <v>699.49214400000005</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3" t="s">
         <v>4</v>
       </c>
-      <c r="C3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C3">
+        <v>36.6</v>
+      </c>
+      <c r="D3">
+        <f>33539.9917667299/1000</f>
+        <v>33.539991766729898</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
       </c>
-      <c r="C4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C4">
+        <v>25.9</v>
+      </c>
+      <c r="D4">
+        <f>23734.5843376586/1000</f>
+        <v>23.734584337658603</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>1</v>
       </c>
       <c r="B5" t="s">
         <v>7</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5">
+        <v>9.6999999999999993</v>
+      </c>
+      <c r="D5">
+        <f>8889.01421140108/1000</f>
+        <v>8.8890142114010793</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2">
+        <v>431.7</v>
+      </c>
+      <c r="D2">
+        <f>C2*B16*1.04</f>
+        <v>699.49214400000005</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3">
+        <v>36.6</v>
+      </c>
+      <c r="D3">
+        <f>B14*B8/1000</f>
+        <v>3.3539991766729851E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4">
+        <v>25.9</v>
+      </c>
+      <c r="D4">
+        <f>B14*B9/1000</f>
+        <v>2.373458433765855E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5">
+        <v>9.6999999999999993</v>
+      </c>
+      <c r="D5">
+        <f>B14*B10/1000</f>
+        <v>8.8890142114010796E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8">
+        <f>C3/(C3+C4+C5)</f>
+        <v>0.50692520775623273</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9">
+        <f>C4/(C3+C4+C5)</f>
+        <v>0.35872576177285315</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10">
+        <f>C5/(C3+C4+C5)</f>
+        <v>0.13434903047091412</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <f>(56990*1.01)/1.9</f>
+        <v>30294.684210526317</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>12</v>
+      </c>
+      <c r="B13">
+        <f>B12*1.04</f>
+        <v>31506.47157894737</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14">
+        <f>B13*2.1/1000</f>
+        <v>66.163590315789477</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16">
+        <v>1.5580000000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>